<commit_message>
Edit report and Create workExperience
</commit_message>
<xml_diff>
--- a/server/storage/private/report/Playtorium_Summary_Leave.xlsx
+++ b/server/storage/private/report/Playtorium_Summary_Leave.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Leave" sheetId="1" r:id="rId1"/>
@@ -203,13 +203,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,6 +268,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -277,25 +283,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -582,7 +582,7 @@
   <dimension ref="B1:BG5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -609,8 +609,8 @@
       <c r="C2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="4" spans="2:59" s="3" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
@@ -628,16 +628,16 @@
       <c r="F4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="7" t="s">
@@ -712,7 +712,7 @@
       <c r="BD4" s="7"/>
       <c r="BE4" s="7"/>
       <c r="BF4" s="7"/>
-      <c r="BG4" s="8" t="s">
+      <c r="BG4" s="16" t="s">
         <v>25</v>
       </c>
     </row>
@@ -722,10 +722,10 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="15"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="4" t="s">
         <v>10</v>
       </c>
@@ -870,17 +870,10 @@
       <c r="BF5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="BG5" s="9"/>
+      <c r="BG5" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
     <mergeCell ref="AU4:AX4"/>
     <mergeCell ref="AY4:BB4"/>
     <mergeCell ref="BC4:BF4"/>
@@ -897,6 +890,13 @@
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:N4"/>
     <mergeCell ref="O4:R4"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>